<commit_message>
set_sprite(texture); growth + collisionbox DB
</commit_message>
<xml_diff>
--- a/db/GENERAL.xlsx
+++ b/db/GENERAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mon\Documents\UOC\TF\Click&amp;Collect TFG\ProjectTF\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDCB582-E534-4934-AB8D-44CB523D7C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B50A840-EAB4-46EF-824F-2BC4C81A9482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{A062384A-F7C0-4E02-B140-8964EB3F575D}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="2" xr2:uid="{A062384A-F7C0-4E02-B140-8964EB3F575D}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="277">
   <si>
     <t>Filename</t>
   </si>
@@ -823,56 +823,59 @@
     <t>whiteTree</t>
   </si>
   <si>
-    <t>stage_1</t>
-  </si>
-  <si>
-    <t>stage_2</t>
-  </si>
-  <si>
-    <t>water_1</t>
-  </si>
-  <si>
-    <t>sun_1</t>
-  </si>
-  <si>
-    <t>water_2</t>
-  </si>
-  <si>
-    <t>sun_2</t>
-  </si>
-  <si>
-    <t>stage_3</t>
-  </si>
-  <si>
-    <t>water_3</t>
-  </si>
-  <si>
-    <t>sun_3</t>
-  </si>
-  <si>
-    <t>stage_4</t>
-  </si>
-  <si>
-    <t>water_4</t>
-  </si>
-  <si>
-    <t>sun_4</t>
-  </si>
-  <si>
-    <t>harvest</t>
-  </si>
-  <si>
-    <t>max_water</t>
-  </si>
-  <si>
-    <t>max_sun</t>
+    <t>water</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>sprite 1 size.x</t>
+  </si>
+  <si>
+    <t>sprite 1 size.y</t>
+  </si>
+  <si>
+    <t>sprite 2 size.x</t>
+  </si>
+  <si>
+    <t>sprite 2 size.y</t>
+  </si>
+  <si>
+    <t>sprite 3 size.x</t>
+  </si>
+  <si>
+    <t>sprite 3 size.y</t>
+  </si>
+  <si>
+    <t>sprite 4 size.x</t>
+  </si>
+  <si>
+    <t>sprite 4 size.y</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>10.05</t>
+  </si>
+  <si>
+    <t>13.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -897,6 +900,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -949,13 +960,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -4505,32 +4517,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E51D7B-EF88-4777-911A-B843F75097D3}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>261</v>
       </c>
       <c r="C1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" t="s">
         <v>263</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>264</v>
-      </c>
-      <c r="E1" t="s">
-        <v>262</v>
       </c>
       <c r="F1" t="s">
         <v>265</v>
@@ -4556,446 +4570,1112 @@
       <c r="M1" t="s">
         <v>272</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2">
+        <v>128</v>
+      </c>
+      <c r="G2">
+        <v>121</v>
+      </c>
+      <c r="H2">
+        <v>255</v>
+      </c>
+      <c r="I2">
+        <v>196</v>
+      </c>
+      <c r="J2">
+        <v>234</v>
+      </c>
+      <c r="K2">
+        <v>196</v>
+      </c>
+      <c r="L2">
+        <v>234</v>
+      </c>
+      <c r="M2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3">
+        <v>128</v>
+      </c>
+      <c r="G3">
+        <v>121</v>
+      </c>
+      <c r="H3">
+        <v>139</v>
+      </c>
+      <c r="I3">
+        <v>160</v>
+      </c>
+      <c r="J3">
+        <v>140</v>
+      </c>
+      <c r="K3">
+        <v>242</v>
+      </c>
+      <c r="L3">
+        <v>140</v>
+      </c>
+      <c r="M3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4">
+        <v>128</v>
+      </c>
+      <c r="G4">
+        <v>121</v>
+      </c>
+      <c r="H4">
+        <v>139</v>
+      </c>
+      <c r="I4">
+        <v>160</v>
+      </c>
+      <c r="J4">
+        <v>140</v>
+      </c>
+      <c r="K4">
+        <v>242</v>
+      </c>
+      <c r="L4">
+        <v>140</v>
+      </c>
+      <c r="M4">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5">
+        <v>128</v>
+      </c>
+      <c r="G5">
+        <v>121</v>
+      </c>
+      <c r="H5">
+        <v>139</v>
+      </c>
+      <c r="I5">
+        <v>160</v>
+      </c>
+      <c r="J5">
+        <v>140</v>
+      </c>
+      <c r="K5">
+        <v>242</v>
+      </c>
+      <c r="L5">
+        <v>140</v>
+      </c>
+      <c r="M5">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6">
+        <v>128</v>
+      </c>
+      <c r="G6">
+        <v>121</v>
+      </c>
+      <c r="H6">
+        <v>139</v>
+      </c>
+      <c r="I6">
+        <v>160</v>
+      </c>
+      <c r="J6">
+        <v>140</v>
+      </c>
+      <c r="K6">
+        <v>242</v>
+      </c>
+      <c r="L6">
+        <v>140</v>
+      </c>
+      <c r="M6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7">
+        <v>128</v>
+      </c>
+      <c r="G7">
+        <v>121</v>
+      </c>
+      <c r="H7">
+        <v>139</v>
+      </c>
+      <c r="I7">
+        <v>160</v>
+      </c>
+      <c r="J7">
+        <v>128</v>
+      </c>
+      <c r="K7">
+        <v>189</v>
+      </c>
+      <c r="L7">
+        <v>182</v>
+      </c>
+      <c r="M7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8">
+        <v>128</v>
+      </c>
+      <c r="G8">
+        <v>121</v>
+      </c>
+      <c r="H8">
+        <v>139</v>
+      </c>
+      <c r="I8">
+        <v>119</v>
+      </c>
+      <c r="J8">
+        <v>139</v>
+      </c>
+      <c r="K8">
+        <v>119</v>
+      </c>
+      <c r="L8">
+        <v>197</v>
+      </c>
+      <c r="M8">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9">
+        <v>128</v>
+      </c>
+      <c r="G9">
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <v>139</v>
+      </c>
+      <c r="I9">
+        <v>90</v>
+      </c>
+      <c r="J9">
+        <v>177</v>
+      </c>
+      <c r="K9">
+        <v>123</v>
+      </c>
+      <c r="L9">
+        <v>177</v>
+      </c>
+      <c r="M9">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>128</v>
+      </c>
+      <c r="G10">
+        <v>121</v>
+      </c>
+      <c r="H10">
+        <v>139</v>
+      </c>
+      <c r="I10">
+        <v>119</v>
+      </c>
+      <c r="J10">
+        <v>139</v>
+      </c>
+      <c r="K10">
+        <v>119</v>
+      </c>
+      <c r="L10">
+        <v>177</v>
+      </c>
+      <c r="M10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11">
+        <v>159</v>
+      </c>
+      <c r="G11">
+        <v>186</v>
+      </c>
+      <c r="H11">
+        <v>220</v>
+      </c>
+      <c r="I11">
+        <v>167</v>
+      </c>
+      <c r="J11">
+        <v>220</v>
+      </c>
+      <c r="K11">
+        <v>189</v>
+      </c>
+      <c r="L11">
+        <v>220</v>
+      </c>
+      <c r="M11">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12">
+        <v>159</v>
+      </c>
+      <c r="G12">
+        <v>186</v>
+      </c>
+      <c r="H12">
+        <v>159</v>
+      </c>
+      <c r="I12">
+        <v>186</v>
+      </c>
+      <c r="J12">
+        <v>163</v>
+      </c>
+      <c r="K12">
+        <v>218</v>
+      </c>
+      <c r="L12">
+        <v>205</v>
+      </c>
+      <c r="M12">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13">
+        <v>159</v>
+      </c>
+      <c r="G13">
+        <v>186</v>
+      </c>
+      <c r="H13">
+        <v>168</v>
+      </c>
+      <c r="I13">
+        <v>195</v>
+      </c>
+      <c r="J13">
+        <v>173</v>
+      </c>
+      <c r="K13">
+        <v>215</v>
+      </c>
+      <c r="L13">
+        <v>203</v>
+      </c>
+      <c r="M13">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14">
+        <v>159</v>
+      </c>
+      <c r="G14">
+        <v>186</v>
+      </c>
+      <c r="H14">
+        <v>168</v>
+      </c>
+      <c r="I14">
+        <v>195</v>
+      </c>
+      <c r="J14" s="6">
+        <v>163</v>
+      </c>
+      <c r="K14">
+        <v>202</v>
+      </c>
+      <c r="L14">
+        <v>220</v>
+      </c>
+      <c r="M14">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15">
+        <v>159</v>
+      </c>
+      <c r="G15">
+        <v>186</v>
+      </c>
+      <c r="H15">
+        <v>242</v>
+      </c>
+      <c r="I15">
+        <v>182</v>
+      </c>
+      <c r="J15">
+        <v>223</v>
+      </c>
+      <c r="K15">
+        <v>235</v>
+      </c>
+      <c r="L15">
+        <v>205</v>
+      </c>
+      <c r="M15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16">
+        <v>159</v>
+      </c>
+      <c r="G16">
+        <v>186</v>
+      </c>
+      <c r="H16">
+        <v>128</v>
+      </c>
+      <c r="I16">
+        <v>160</v>
+      </c>
+      <c r="J16">
+        <v>140</v>
+      </c>
+      <c r="K16">
+        <v>242</v>
+      </c>
+      <c r="L16">
+        <v>140</v>
+      </c>
+      <c r="M16">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17">
+        <v>159</v>
+      </c>
+      <c r="G17">
+        <v>186</v>
+      </c>
+      <c r="H17">
+        <v>242</v>
+      </c>
+      <c r="I17">
+        <v>182</v>
+      </c>
+      <c r="J17">
+        <v>231</v>
+      </c>
+      <c r="K17">
+        <v>241</v>
+      </c>
+      <c r="L17">
+        <v>231</v>
+      </c>
+      <c r="M17">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18">
+        <v>128</v>
+      </c>
+      <c r="G18">
+        <v>203</v>
+      </c>
+      <c r="H18">
+        <v>242</v>
+      </c>
+      <c r="I18">
+        <v>182</v>
+      </c>
+      <c r="J18">
+        <v>242</v>
+      </c>
+      <c r="K18">
+        <v>182</v>
+      </c>
+      <c r="L18">
+        <v>223</v>
+      </c>
+      <c r="M18">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19">
+        <v>159</v>
+      </c>
+      <c r="G19">
+        <v>186</v>
+      </c>
+      <c r="H19">
+        <v>168</v>
+      </c>
+      <c r="I19">
+        <v>195</v>
+      </c>
+      <c r="J19">
+        <v>168</v>
+      </c>
+      <c r="K19">
+        <v>211</v>
+      </c>
+      <c r="L19">
+        <v>203</v>
+      </c>
+      <c r="M19">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>273</v>
       </c>
-      <c r="P1" t="s">
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20">
+        <v>140</v>
+      </c>
+      <c r="G20">
+        <v>242</v>
+      </c>
+      <c r="H20">
+        <v>269</v>
+      </c>
+      <c r="I20">
+        <v>324</v>
+      </c>
+      <c r="J20">
+        <v>461</v>
+      </c>
+      <c r="K20">
+        <v>491</v>
+      </c>
+      <c r="L20">
+        <v>461</v>
+      </c>
+      <c r="M20">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>274</v>
       </c>
-      <c r="Q1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <f>SUM(C2,F2,I2,L2)</f>
-        <v>4</v>
-      </c>
-      <c r="Q2">
-        <f>SUM(D2,G2,J2,M2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>235</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P28" si="0">SUM(C3,F3,I3,L3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q28" si="1">SUM(D3,G3,J3,M3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>236</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>237</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>239</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>238</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>240</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>241</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21">
+        <v>140</v>
+      </c>
+      <c r="G21">
         <v>242</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>243</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>244</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>245</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>246</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>247</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>250</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>251</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>249</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>248</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>252</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>2</v>
-      </c>
-      <c r="M20">
-        <v>3</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
+      <c r="H21">
+        <v>269</v>
+      </c>
+      <c r="I21">
+        <v>324</v>
+      </c>
+      <c r="J21">
+        <v>461</v>
+      </c>
+      <c r="K21">
+        <v>491</v>
+      </c>
+      <c r="L21">
+        <v>461</v>
+      </c>
+      <c r="M21">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22">
+        <v>140</v>
+      </c>
+      <c r="G22">
+        <v>242</v>
+      </c>
+      <c r="H22">
+        <v>269</v>
+      </c>
+      <c r="I22">
+        <v>324</v>
+      </c>
+      <c r="J22">
+        <v>292</v>
+      </c>
+      <c r="K22">
+        <v>317</v>
+      </c>
+      <c r="L22">
+        <v>292</v>
+      </c>
+      <c r="M22">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
         <v>7</v>
       </c>
-      <c r="Q20">
-        <f t="shared" si="1"/>
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23">
+        <v>140</v>
+      </c>
+      <c r="G23">
+        <v>242</v>
+      </c>
+      <c r="H23">
+        <v>322</v>
+      </c>
+      <c r="I23">
+        <v>218</v>
+      </c>
+      <c r="J23">
+        <v>461</v>
+      </c>
+      <c r="K23">
+        <v>324</v>
+      </c>
+      <c r="L23">
+        <v>461</v>
+      </c>
+      <c r="M23">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>273</v>
+      </c>
+      <c r="E24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24">
+        <v>140</v>
+      </c>
+      <c r="G24">
+        <v>242</v>
+      </c>
+      <c r="H24">
+        <v>269</v>
+      </c>
+      <c r="I24">
+        <v>324</v>
+      </c>
+      <c r="J24">
+        <v>461</v>
+      </c>
+      <c r="K24">
+        <v>491</v>
+      </c>
+      <c r="L24">
+        <v>461</v>
+      </c>
+      <c r="M24">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25">
+        <v>140</v>
+      </c>
+      <c r="G25">
+        <v>242</v>
+      </c>
+      <c r="H25">
+        <v>269</v>
+      </c>
+      <c r="I25">
+        <v>324</v>
+      </c>
+      <c r="J25">
+        <v>461</v>
+      </c>
+      <c r="K25">
+        <v>491</v>
+      </c>
+      <c r="L25">
+        <v>461</v>
+      </c>
+      <c r="M25">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>254</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>257</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>253</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>255</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>258</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>259</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>273</v>
+      </c>
+      <c r="E26" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26">
+        <v>140</v>
+      </c>
+      <c r="G26">
+        <v>242</v>
+      </c>
+      <c r="H26">
+        <v>269</v>
+      </c>
+      <c r="I26">
+        <v>324</v>
+      </c>
+      <c r="J26">
+        <v>461</v>
+      </c>
+      <c r="K26">
+        <v>491</v>
+      </c>
+      <c r="L26">
+        <v>461</v>
+      </c>
+      <c r="M26">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>256</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>273</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27">
+        <v>140</v>
+      </c>
+      <c r="G27">
+        <v>242</v>
+      </c>
+      <c r="H27">
+        <v>269</v>
+      </c>
+      <c r="I27">
+        <v>324</v>
+      </c>
+      <c r="J27">
+        <v>461</v>
+      </c>
+      <c r="K27">
+        <v>307</v>
+      </c>
+      <c r="L27">
+        <v>461</v>
+      </c>
+      <c r="M27">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>260</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>273</v>
+      </c>
+      <c r="E28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28">
+        <v>140</v>
+      </c>
+      <c r="G28">
+        <v>242</v>
+      </c>
+      <c r="H28">
+        <v>269</v>
+      </c>
+      <c r="I28">
+        <v>324</v>
+      </c>
+      <c r="J28">
+        <v>461</v>
+      </c>
+      <c r="K28">
+        <v>491</v>
+      </c>
+      <c r="L28">
+        <v>461</v>
+      </c>
+      <c r="M28">
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>